<commit_message>
Final version. Ready to merge
</commit_message>
<xml_diff>
--- a/Line_data.xlsx
+++ b/Line_data.xlsx
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,10 +645,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F2">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G2">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H2">
         <v>0.34200000000000003</v>
@@ -657,12 +657,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J2">
-        <f>5.2*0.8</f>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K2">
-        <f>5.2*0.6</f>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L2">
         <v>10000</v>
@@ -674,10 +672,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O2">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P2">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q2">
         <v>8500</v>
@@ -689,12 +687,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T2">
-        <f>5.2*0.8</f>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U2">
-        <f>5.2*0.6</f>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V2">
         <v>15000</v>
@@ -706,12 +702,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y2">
-        <f>8.1*0.8</f>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z2">
-        <f>8.1*0.6</f>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA2">
         <v>35000</v>
@@ -740,10 +734,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F3">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G3">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H3">
         <v>0.34200000000000003</v>
@@ -752,12 +746,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J10" si="0">5.2*0.8</f>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K10" si="1">5.2*0.6</f>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L3">
         <v>10000</v>
@@ -769,10 +761,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O3">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P3">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q3">
         <v>8500</v>
@@ -784,12 +776,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T39" si="2">5.2*0.8</f>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U39" si="3">5.2*0.6</f>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V3">
         <v>15000</v>
@@ -801,12 +791,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y39" si="4">8.1*0.8</f>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z39" si="5">8.1*0.6</f>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA3">
         <v>35000</v>
@@ -835,10 +823,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F4">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>0.34200000000000003</v>
@@ -847,12 +835,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L4">
         <v>10000</v>
@@ -864,10 +850,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O4">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P4">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q4">
         <v>8500</v>
@@ -879,12 +865,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T4">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U4">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V4">
         <v>15000</v>
@@ -896,12 +880,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA4">
         <v>35000</v>
@@ -930,10 +912,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F5">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G5">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H5">
         <v>0.34200000000000003</v>
@@ -942,12 +924,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L5">
         <v>10000</v>
@@ -959,10 +939,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O5">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P5">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q5">
         <v>8500</v>
@@ -974,12 +954,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T5">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U5">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V5">
         <v>15000</v>
@@ -991,12 +969,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA5">
         <v>35000</v>
@@ -1025,10 +1001,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F6">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H6">
         <v>0.34200000000000003</v>
@@ -1037,12 +1013,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L6">
         <v>10000</v>
@@ -1054,10 +1028,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O6">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P6">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q6">
         <v>8500</v>
@@ -1069,12 +1043,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T6">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U6">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V6">
         <v>15000</v>
@@ -1086,12 +1058,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA6">
         <v>35000</v>
@@ -1120,10 +1090,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F7">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G7">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H7">
         <v>0.34200000000000003</v>
@@ -1132,12 +1102,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L7">
         <v>10000</v>
@@ -1149,10 +1117,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O7">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P7">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q7">
         <v>8500</v>
@@ -1164,12 +1132,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T7">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U7">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V7">
         <v>15000</v>
@@ -1181,12 +1147,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA7">
         <v>35000</v>
@@ -1215,10 +1179,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F8">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G8">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H8">
         <v>0.34200000000000003</v>
@@ -1227,12 +1191,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L8">
         <v>10000</v>
@@ -1244,10 +1206,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O8">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P8">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q8">
         <v>8500</v>
@@ -1259,12 +1221,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T8">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U8">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V8">
         <v>15000</v>
@@ -1276,12 +1236,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA8">
         <v>35000</v>
@@ -1310,10 +1268,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F9">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H9">
         <v>0.34200000000000003</v>
@@ -1322,12 +1280,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L9">
         <v>10000</v>
@@ -1339,10 +1295,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O9">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P9">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q9">
         <v>8500</v>
@@ -1354,12 +1310,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T9">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U9">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V9">
         <v>15000</v>
@@ -1371,12 +1325,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA9">
         <v>35000</v>
@@ -1405,10 +1357,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="F10">
-        <v>2.72</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>2.04</v>
+        <v>20</v>
       </c>
       <c r="H10">
         <v>0.34200000000000003</v>
@@ -1417,12 +1369,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
-        <v>4.16</v>
+        <v>30</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <v>30</v>
       </c>
       <c r="L10">
         <v>10000</v>
@@ -1434,10 +1384,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O10">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P10">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q10">
         <v>8500</v>
@@ -1449,12 +1399,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T10">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U10">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V10">
         <v>15000</v>
@@ -1466,12 +1414,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA10">
         <v>35000</v>
@@ -1500,10 +1446,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O11">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P11">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q11">
         <v>8500</v>
@@ -1515,12 +1461,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U11">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V11">
         <v>15000</v>
@@ -1532,12 +1476,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA11">
         <v>35000</v>
@@ -1566,10 +1508,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O12">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P12">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q12">
         <v>8500</v>
@@ -1581,12 +1523,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U12">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V12">
         <v>15000</v>
@@ -1598,12 +1538,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA12">
         <v>35000</v>
@@ -1632,10 +1570,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O13">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P13">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q13">
         <v>8500</v>
@@ -1647,12 +1585,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U13">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V13">
         <v>15000</v>
@@ -1664,12 +1600,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA13">
         <v>35000</v>
@@ -1698,10 +1632,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O14">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P14">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q14">
         <v>8500</v>
@@ -1713,12 +1647,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U14">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V14">
         <v>15000</v>
@@ -1730,12 +1662,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA14">
         <v>35000</v>
@@ -1764,10 +1694,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O15">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P15">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q15">
         <v>8500</v>
@@ -1779,12 +1709,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V15">
         <v>15000</v>
@@ -1796,12 +1724,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA15">
         <v>35000</v>
@@ -1830,10 +1756,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O16">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P16">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q16">
         <v>8500</v>
@@ -1845,12 +1771,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T16">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U16">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V16">
         <v>15000</v>
@@ -1862,12 +1786,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA16">
         <v>35000</v>
@@ -1896,10 +1818,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O17">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P17">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q17">
         <v>8500</v>
@@ -1911,12 +1833,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T17">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U17">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V17">
         <v>15000</v>
@@ -1928,12 +1848,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA17">
         <v>35000</v>
@@ -1962,10 +1880,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O18">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P18">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q18">
         <v>8500</v>
@@ -1977,12 +1895,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T18">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U18">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V18">
         <v>15000</v>
@@ -1994,12 +1910,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA18">
         <v>35000</v>
@@ -2028,10 +1942,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O19">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P19">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q19">
         <v>8500</v>
@@ -2043,12 +1957,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T19">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U19">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V19">
         <v>15000</v>
@@ -2060,12 +1972,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA19">
         <v>35000</v>
@@ -2094,10 +2004,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O20">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P20">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q20">
         <v>8500</v>
@@ -2109,12 +2019,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T20">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U20">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V20">
         <v>15000</v>
@@ -2126,12 +2034,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA20">
         <v>35000</v>
@@ -2160,10 +2066,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O21">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P21">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q21">
         <v>8500</v>
@@ -2175,12 +2081,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T21">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U21">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V21">
         <v>15000</v>
@@ -2192,12 +2096,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA21">
         <v>35000</v>
@@ -2226,10 +2128,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O22">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P22">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q22">
         <v>8500</v>
@@ -2241,12 +2143,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T22">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U22">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V22">
         <v>15000</v>
@@ -2258,12 +2158,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA22">
         <v>35000</v>
@@ -2292,10 +2190,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O23">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P23">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q23">
         <v>8500</v>
@@ -2307,12 +2205,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T23">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U23">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V23">
         <v>15000</v>
@@ -2324,12 +2220,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA23">
         <v>35000</v>
@@ -2358,10 +2252,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O24">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P24">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q24">
         <v>8500</v>
@@ -2373,12 +2267,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T24">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U24">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V24">
         <v>15000</v>
@@ -2390,12 +2282,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA24">
         <v>35000</v>
@@ -2424,10 +2314,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O25">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P25">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q25">
         <v>8500</v>
@@ -2439,12 +2329,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T25">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U25">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V25">
         <v>15000</v>
@@ -2456,12 +2344,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA25">
         <v>35000</v>
@@ -2490,10 +2376,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O26">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P26">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q26">
         <v>8500</v>
@@ -2505,12 +2391,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T26">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U26">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V26">
         <v>15000</v>
@@ -2522,12 +2406,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA26">
         <v>35000</v>
@@ -2556,10 +2438,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O27">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P27">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q27">
         <v>8500</v>
@@ -2571,12 +2453,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T27">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U27">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V27">
         <v>15000</v>
@@ -2588,12 +2468,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA27">
         <v>35000</v>
@@ -2622,10 +2500,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O28">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P28">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q28">
         <v>8500</v>
@@ -2637,12 +2515,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T28">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U28">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V28">
         <v>15000</v>
@@ -2654,12 +2530,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA28">
         <v>35000</v>
@@ -2688,10 +2562,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O29">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P29">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q29">
         <v>8500</v>
@@ -2703,12 +2577,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T29">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U29">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V29">
         <v>15000</v>
@@ -2720,12 +2592,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA29">
         <v>35000</v>
@@ -2754,10 +2624,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O30">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P30">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q30">
         <v>8500</v>
@@ -2769,12 +2639,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T30">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U30">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V30">
         <v>15000</v>
@@ -2786,12 +2654,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA30">
         <v>35000</v>
@@ -2820,10 +2686,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O31">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P31">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q31">
         <v>8500</v>
@@ -2835,12 +2701,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T31">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U31">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V31">
         <v>15000</v>
@@ -2852,12 +2716,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA31">
         <v>35000</v>
@@ -2886,10 +2748,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O32">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P32">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q32">
         <v>8500</v>
@@ -2901,12 +2763,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T32">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U32">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V32">
         <v>15000</v>
@@ -2918,12 +2778,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA32">
         <v>35000</v>
@@ -2952,10 +2810,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O33">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P33">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q33">
         <v>8500</v>
@@ -2967,12 +2825,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T33">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U33">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V33">
         <v>15000</v>
@@ -2984,12 +2840,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA33">
         <v>35000</v>
@@ -3018,10 +2872,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O34">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P34">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q34">
         <v>8500</v>
@@ -3033,12 +2887,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T34">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U34">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V34">
         <v>15000</v>
@@ -3050,12 +2902,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA34">
         <v>35000</v>
@@ -3084,10 +2934,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O35">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P35">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q35">
         <v>8500</v>
@@ -3099,12 +2949,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T35">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U35">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V35">
         <v>15000</v>
@@ -3116,12 +2964,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA35">
         <v>35000</v>
@@ -3150,10 +2996,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O36">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P36">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q36">
         <v>8500</v>
@@ -3165,12 +3011,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T36">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U36">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V36">
         <v>15000</v>
@@ -3182,12 +3026,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA36">
         <v>35000</v>
@@ -3216,10 +3058,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O37">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P37">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q37">
         <v>8500</v>
@@ -3231,12 +3073,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T37">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U37">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V37">
         <v>15000</v>
@@ -3248,12 +3088,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA37">
         <v>35000</v>
@@ -3282,10 +3120,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O38">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P38">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q38">
         <v>8500</v>
@@ -3297,12 +3135,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T38">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U38">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V38">
         <v>15000</v>
@@ -3314,12 +3150,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA38">
         <v>35000</v>
@@ -3348,10 +3182,10 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="O39">
-        <v>2.72</v>
+        <v>21</v>
       </c>
       <c r="P39">
-        <v>2.04</v>
+        <v>21</v>
       </c>
       <c r="Q39">
         <v>8500</v>
@@ -3363,12 +3197,10 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="T39">
-        <f t="shared" si="2"/>
-        <v>4.16</v>
+        <v>22</v>
       </c>
       <c r="U39">
-        <f t="shared" si="3"/>
-        <v>3.12</v>
+        <v>22</v>
       </c>
       <c r="V39">
         <v>15000</v>
@@ -3380,12 +3212,10 @@
         <v>0.20399999999999999</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="4"/>
-        <v>6.48</v>
+        <v>23</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="5"/>
-        <v>4.8599999999999994</v>
+        <v>23</v>
       </c>
       <c r="AA39">
         <v>35000</v>

</xml_diff>